<commit_message>
added PWM DAC CTL
</commit_message>
<xml_diff>
--- a/Generate Files/Bill of Materials/Bill of Materials-H18-002.xlsx
+++ b/Generate Files/Bill of Materials/Bill of Materials-H18-002.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="132">
   <si>
     <t>Comment</t>
   </si>
@@ -52,7 +52,7 @@
     <t>100p</t>
   </si>
   <si>
-    <t>C2, C5, C6, C12, C29, C30, C32</t>
+    <t>C2, C5, C6, C12, C30, C32</t>
   </si>
   <si>
     <t>100n</t>
@@ -64,7 +64,7 @@
     <t>caps, caps, caps, casp, caps</t>
   </si>
   <si>
-    <t>47n NPO</t>
+    <t>15n NPO</t>
   </si>
   <si>
     <t>C7</t>
@@ -76,7 +76,7 @@
     <t>C8</t>
   </si>
   <si>
-    <t>100n NPO</t>
+    <t>68n NPO</t>
   </si>
   <si>
     <t>C9</t>
@@ -91,10 +91,10 @@
     <t>10n</t>
   </si>
   <si>
-    <t>C13, C16, C17, C27</t>
-  </si>
-  <si>
-    <t>casp</t>
+    <t>C13, C16, C17, C27, C29</t>
+  </si>
+  <si>
+    <t>casp, casp, casp, casp, caps</t>
   </si>
   <si>
     <t>470p</t>
@@ -265,31 +265,37 @@
     <t>47k</t>
   </si>
   <si>
-    <t>R2, R16, R24, R25, R34</t>
+    <t>R2, R16, R24, R25, R31, R34</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>0603R</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>5k1</t>
+  </si>
+  <si>
+    <t>R5</t>
   </si>
   <si>
     <t>51</t>
   </si>
   <si>
-    <t>R3, R4</t>
-  </si>
-  <si>
-    <t>0603R</t>
-  </si>
-  <si>
-    <t>5k1</t>
-  </si>
-  <si>
-    <t>R5</t>
-  </si>
-  <si>
     <t>R6, R9, R13, R19, R21, R27, R28, R29, R40</t>
   </si>
   <si>
     <t>1k</t>
   </si>
   <si>
-    <t>R7, R8, R10, R11</t>
+    <t>R7, R8, R10, R11, R42</t>
   </si>
   <si>
     <t>4k7</t>
@@ -328,12 +334,6 @@
     <t>R30, R41</t>
   </si>
   <si>
-    <t>10k</t>
-  </si>
-  <si>
-    <t>R31</t>
-  </si>
-  <si>
     <t>22k</t>
   </si>
   <si>
@@ -350,6 +350,9 @@
   </si>
   <si>
     <t>R36</t>
+  </si>
+  <si>
+    <t>R43</t>
   </si>
   <si>
     <t>MIC5207BM5</t>
@@ -770,7 +773,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -836,7 +839,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -956,7 +959,7 @@
         <v>26</v>
       </c>
       <c r="F9" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1336,7 +1339,7 @@
         <v>81</v>
       </c>
       <c r="F28" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1356,21 +1359,21 @@
         <v>81</v>
       </c>
       <c r="F29" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>78</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>81</v>
@@ -1381,7 +1384,7 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>78</v>
@@ -1396,7 +1399,7 @@
         <v>81</v>
       </c>
       <c r="F31" s="3">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1416,7 +1419,7 @@
         <v>81</v>
       </c>
       <c r="F32" s="3">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1436,7 +1439,7 @@
         <v>81</v>
       </c>
       <c r="F33" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1456,7 +1459,7 @@
         <v>81</v>
       </c>
       <c r="F34" s="3">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1476,7 +1479,7 @@
         <v>81</v>
       </c>
       <c r="F35" s="3">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1496,7 +1499,7 @@
         <v>81</v>
       </c>
       <c r="F36" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1536,7 +1539,7 @@
         <v>81</v>
       </c>
       <c r="F38" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1556,7 +1559,7 @@
         <v>81</v>
       </c>
       <c r="F39" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1621,59 +1624,59 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>114</v>
-      </c>
       <c r="D43" s="2" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>112</v>
+        <v>81</v>
       </c>
       <c r="F43" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B44" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>119</v>
-      </c>
       <c r="E44" s="2" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="F44" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E45" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>125</v>
       </c>
       <c r="F45" s="3">
         <v>1</v>
@@ -1681,21 +1684,41 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="F46" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="B47" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="C47" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E46" s="2" t="s">
+      <c r="D47" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="F46" s="3">
+      <c r="E47" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F47" s="3">
         <v>1</v>
       </c>
     </row>

</xml_diff>